<commit_message>
2B math p. 4, 5
</commit_message>
<xml_diff>
--- a/block 3 grades.xlsx
+++ b/block 3 grades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15120" windowHeight="7545" tabRatio="917" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15120" windowHeight="7545" tabRatio="917" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2A SC" sheetId="2" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="467">
   <si>
     <t>9NO AÑO "B" (BÁSICA SUPERIOR)</t>
   </si>
@@ -1461,6 +1461,12 @@
   </si>
   <si>
     <t>santa claus 13/12/2012</t>
+  </si>
+  <si>
+    <t>p. 5 14/12/2012</t>
+  </si>
+  <si>
+    <t>p. 4, 5 14/12/2012</t>
   </si>
 </sst>
 </file>
@@ -24543,11 +24549,11 @@
   <dimension ref="A1:AH200"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="D4" sqref="D4"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Z9" sqref="Z9"/>
+      <selection pane="bottomRight" activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -24615,7 +24621,7 @@
       <c r="AF3" s="12"/>
       <c r="AG3" s="12"/>
     </row>
-    <row r="4" spans="1:34" s="15" customFormat="1" ht="179.25">
+    <row r="4" spans="1:34" s="15" customFormat="1" ht="178.5">
       <c r="A4" s="14"/>
       <c r="D4" s="15" t="s">
         <v>436</v>
@@ -25922,7 +25928,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z23" s="34"/>
+      <c r="Z23" s="78" t="s">
+        <v>453</v>
+      </c>
       <c r="AA23" s="34"/>
       <c r="AB23" s="34"/>
       <c r="AC23" s="35" t="e">
@@ -28804,11 +28812,11 @@
   <dimension ref="A1:AH200"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="D4" sqref="D4"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -28876,7 +28884,7 @@
       <c r="AF3" s="12"/>
       <c r="AG3" s="12"/>
     </row>
-    <row r="4" spans="1:34" s="15" customFormat="1" ht="179.25">
+    <row r="4" spans="1:34" s="15" customFormat="1" ht="178.5">
       <c r="A4" s="14"/>
       <c r="D4" s="15" t="s">
         <v>429</v>
@@ -29093,14 +29101,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z8" s="34" t="s">
-        <v>453</v>
+      <c r="Z8" s="34">
+        <v>8.6</v>
       </c>
       <c r="AA8" s="34"/>
       <c r="AB8" s="34"/>
-      <c r="AC8" s="35" t="e">
+      <c r="AC8" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>8.6</v>
       </c>
       <c r="AD8" s="36" t="e">
         <f t="shared" ref="AD8:AD39" si="4">TRUNC(AVERAGE(M8,U8,Y8,AC8),2)</f>
@@ -29167,12 +29175,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z9" s="34"/>
+      <c r="Z9" s="34">
+        <v>0</v>
+      </c>
       <c r="AA9" s="34"/>
       <c r="AB9" s="34"/>
-      <c r="AC9" s="35" t="e">
+      <c r="AC9" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AD9" s="36" t="e">
         <f t="shared" si="4"/>
@@ -29313,12 +29323,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z11" s="34"/>
+      <c r="Z11" s="77">
+        <v>7.6</v>
+      </c>
       <c r="AA11" s="34"/>
       <c r="AB11" s="34"/>
-      <c r="AC11" s="35" t="e">
+      <c r="AC11" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>7.6</v>
       </c>
       <c r="AD11" s="36" t="e">
         <f t="shared" si="4"/>
@@ -29459,12 +29471,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z13" s="34"/>
+      <c r="Z13" s="34">
+        <v>0</v>
+      </c>
       <c r="AA13" s="34"/>
       <c r="AB13" s="34"/>
-      <c r="AC13" s="35" t="e">
+      <c r="AC13" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AD13" s="36" t="e">
         <f t="shared" si="4"/>
@@ -29531,12 +29545,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z14" s="34"/>
+      <c r="Z14" s="34">
+        <v>0</v>
+      </c>
       <c r="AA14" s="34"/>
       <c r="AB14" s="34"/>
-      <c r="AC14" s="35" t="e">
+      <c r="AC14" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AD14" s="36" t="e">
         <f t="shared" si="4"/>
@@ -29603,12 +29619,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z15" s="34"/>
+      <c r="Z15" s="34">
+        <v>0</v>
+      </c>
       <c r="AA15" s="34"/>
       <c r="AB15" s="34"/>
-      <c r="AC15" s="35" t="e">
+      <c r="AC15" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AD15" s="36" t="e">
         <f t="shared" si="4"/>
@@ -29675,12 +29693,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z16" s="34"/>
+      <c r="Z16" s="34">
+        <v>0</v>
+      </c>
       <c r="AA16" s="34"/>
       <c r="AB16" s="34"/>
-      <c r="AC16" s="35" t="e">
+      <c r="AC16" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AD16" s="36" t="e">
         <f t="shared" si="4"/>
@@ -29895,12 +29915,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z19" s="34"/>
+      <c r="Z19" s="34">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
-      <c r="AC19" s="35" t="e">
+      <c r="AC19" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="AD19" s="36" t="e">
         <f t="shared" si="4"/>
@@ -29967,7 +29989,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z20" s="34"/>
+      <c r="Z20" s="77" t="s">
+        <v>453</v>
+      </c>
       <c r="AA20" s="34"/>
       <c r="AB20" s="34"/>
       <c r="AC20" s="35" t="e">
@@ -30261,12 +30285,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z24" s="34"/>
+      <c r="Z24" s="34">
+        <v>0</v>
+      </c>
       <c r="AA24" s="34"/>
       <c r="AB24" s="34"/>
-      <c r="AC24" s="35" t="e">
+      <c r="AC24" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AD24" s="36" t="e">
         <f t="shared" si="4"/>
@@ -30333,12 +30359,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z25" s="34"/>
+      <c r="Z25" s="77">
+        <v>7</v>
+      </c>
       <c r="AA25" s="34"/>
       <c r="AB25" s="34"/>
-      <c r="AC25" s="35" t="e">
+      <c r="AC25" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>7</v>
       </c>
       <c r="AD25" s="36" t="e">
         <f t="shared" si="4"/>
@@ -30553,12 +30581,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z28" s="34"/>
+      <c r="Z28" s="77">
+        <v>7</v>
+      </c>
       <c r="AA28" s="34"/>
       <c r="AB28" s="34"/>
-      <c r="AC28" s="35" t="e">
+      <c r="AC28" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>7</v>
       </c>
       <c r="AD28" s="36" t="e">
         <f t="shared" si="4"/>
@@ -30699,12 +30729,14 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z30" s="34"/>
+      <c r="Z30" s="34">
+        <v>0</v>
+      </c>
       <c r="AA30" s="34"/>
       <c r="AB30" s="34"/>
-      <c r="AC30" s="35" t="e">
+      <c r="AC30" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AD30" s="36" t="e">
         <f t="shared" si="4"/>
@@ -41223,7 +41255,7 @@
       <c r="AF3" s="12"/>
       <c r="AG3" s="12"/>
     </row>
-    <row r="4" spans="1:34" s="15" customFormat="1" ht="126">
+    <row r="4" spans="1:34" s="15" customFormat="1" ht="125.25">
       <c r="A4" s="14"/>
       <c r="M4" s="16"/>
       <c r="N4" s="15" t="s">
@@ -45377,12 +45409,12 @@
   </sheetPr>
   <dimension ref="A1:AH200"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="N6" sqref="N6:T6"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -45452,6 +45484,9 @@
     </row>
     <row r="4" spans="1:34" s="15" customFormat="1" ht="109.5">
       <c r="A4" s="14"/>
+      <c r="D4" s="15" t="s">
+        <v>465</v>
+      </c>
       <c r="M4" s="16"/>
       <c r="N4" s="15" t="s">
         <v>458</v>
@@ -45547,7 +45582,9 @@
       <c r="C7" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="34">
+        <v>10</v>
+      </c>
       <c r="E7" s="34"/>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
@@ -45556,9 +45593,9 @@
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
       <c r="L7" s="34"/>
-      <c r="M7" s="35" t="e">
+      <c r="M7" s="35">
         <f>TRUNC(AVERAGE(D7:L7),2)</f>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="N7" s="34">
         <v>10</v>
@@ -45615,7 +45652,9 @@
       <c r="C8" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="34">
+        <v>10</v>
+      </c>
       <c r="E8" s="34"/>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
@@ -45624,9 +45663,9 @@
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
-      <c r="M8" s="35" t="e">
+      <c r="M8" s="35">
         <f t="shared" ref="M8:M39" si="2">TRUNC(AVERAGE(D8:L8),2)</f>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="N8" s="34">
         <v>9.5</v>
@@ -45683,7 +45722,9 @@
       <c r="C9" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="34">
+        <v>10</v>
+      </c>
       <c r="E9" s="34"/>
       <c r="F9" s="34"/>
       <c r="G9" s="34"/>
@@ -45692,9 +45733,9 @@
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
-      <c r="M9" s="35" t="e">
+      <c r="M9" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="N9" s="34">
         <v>9</v>
@@ -45751,7 +45792,9 @@
       <c r="C10" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="34">
+        <v>10</v>
+      </c>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
@@ -45760,9 +45803,9 @@
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
-      <c r="M10" s="35" t="e">
+      <c r="M10" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="N10" s="34">
         <v>9</v>
@@ -45819,7 +45862,9 @@
       <c r="C11" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="34"/>
+      <c r="D11" s="34">
+        <v>10</v>
+      </c>
       <c r="E11" s="34"/>
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
@@ -45828,9 +45873,9 @@
       <c r="J11" s="34"/>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
-      <c r="M11" s="35" t="e">
+      <c r="M11" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="N11" s="34">
         <v>9.5</v>
@@ -45887,7 +45932,9 @@
       <c r="C12" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="34">
+        <v>10</v>
+      </c>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
       <c r="G12" s="34"/>
@@ -45896,9 +45943,9 @@
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
-      <c r="M12" s="35" t="e">
+      <c r="M12" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="N12" s="34">
         <v>9</v>
@@ -45955,7 +46002,9 @@
       <c r="C13" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="34">
+        <v>10</v>
+      </c>
       <c r="E13" s="34"/>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
@@ -45964,9 +46013,9 @@
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
-      <c r="M13" s="35" t="e">
+      <c r="M13" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="N13" s="34">
         <v>8</v>
@@ -46023,7 +46072,9 @@
       <c r="C14" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="34"/>
+      <c r="D14" s="34">
+        <v>9</v>
+      </c>
       <c r="E14" s="34"/>
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
@@ -46032,9 +46083,9 @@
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
-      <c r="M14" s="35" t="e">
+      <c r="M14" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>9</v>
       </c>
       <c r="N14" s="34">
         <v>9.5</v>
@@ -46091,7 +46142,9 @@
       <c r="C15" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="34"/>
+      <c r="D15" s="34">
+        <v>9</v>
+      </c>
       <c r="E15" s="34"/>
       <c r="F15" s="34"/>
       <c r="G15" s="34"/>
@@ -46100,9 +46153,9 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
-      <c r="M15" s="35" t="e">
+      <c r="M15" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>9</v>
       </c>
       <c r="N15" s="34">
         <v>9</v>
@@ -46159,7 +46212,9 @@
       <c r="C16" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="34"/>
+      <c r="D16" s="34" t="s">
+        <v>421</v>
+      </c>
       <c r="E16" s="34"/>
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
@@ -46227,7 +46282,9 @@
       <c r="C17" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="34"/>
+      <c r="D17" s="34">
+        <v>9</v>
+      </c>
       <c r="E17" s="34"/>
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
@@ -46236,9 +46293,9 @@
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
-      <c r="M17" s="35" t="e">
+      <c r="M17" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>9</v>
       </c>
       <c r="N17" s="34">
         <v>10</v>
@@ -46295,7 +46352,9 @@
       <c r="C18" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="34"/>
+      <c r="D18" s="34">
+        <v>10</v>
+      </c>
       <c r="E18" s="34"/>
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
@@ -46304,9 +46363,9 @@
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
       <c r="L18" s="34"/>
-      <c r="M18" s="35" t="e">
+      <c r="M18" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="N18" s="34">
         <v>9</v>
@@ -46363,7 +46422,9 @@
       <c r="C19" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="34"/>
+      <c r="D19" s="34">
+        <v>10</v>
+      </c>
       <c r="E19" s="34"/>
       <c r="F19" s="34"/>
       <c r="G19" s="34"/>
@@ -46372,9 +46433,9 @@
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
       <c r="L19" s="34"/>
-      <c r="M19" s="35" t="e">
+      <c r="M19" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="N19" s="34">
         <v>9</v>
@@ -46431,7 +46492,9 @@
       <c r="C20" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="34"/>
+      <c r="D20" s="34">
+        <v>7</v>
+      </c>
       <c r="E20" s="34"/>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
@@ -46440,9 +46503,9 @@
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
       <c r="L20" s="34"/>
-      <c r="M20" s="35" t="e">
+      <c r="M20" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>7</v>
       </c>
       <c r="N20" s="34">
         <v>9.5</v>
@@ -46499,7 +46562,9 @@
       <c r="C21" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="34"/>
+      <c r="D21" s="34">
+        <v>9.5</v>
+      </c>
       <c r="E21" s="34"/>
       <c r="F21" s="34"/>
       <c r="G21" s="34"/>
@@ -46508,9 +46573,9 @@
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
       <c r="L21" s="34"/>
-      <c r="M21" s="35" t="e">
+      <c r="M21" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>9.5</v>
       </c>
       <c r="N21" s="34">
         <v>9.5</v>
@@ -46567,7 +46632,9 @@
       <c r="C22" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="34"/>
+      <c r="D22" s="34">
+        <v>9</v>
+      </c>
       <c r="E22" s="34"/>
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
@@ -46576,9 +46643,9 @@
       <c r="J22" s="34"/>
       <c r="K22" s="34"/>
       <c r="L22" s="34"/>
-      <c r="M22" s="35" t="e">
+      <c r="M22" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>9</v>
       </c>
       <c r="N22" s="34">
         <v>9.5</v>
@@ -46635,7 +46702,9 @@
       <c r="C23" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="34"/>
+      <c r="D23" s="34">
+        <v>10</v>
+      </c>
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
@@ -46644,9 +46713,9 @@
       <c r="J23" s="34"/>
       <c r="K23" s="34"/>
       <c r="L23" s="34"/>
-      <c r="M23" s="35" t="e">
+      <c r="M23" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="N23" s="34">
         <v>9.5</v>
@@ -46703,7 +46772,9 @@
       <c r="C24" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="34"/>
+      <c r="D24" s="34">
+        <v>1</v>
+      </c>
       <c r="E24" s="34"/>
       <c r="F24" s="34"/>
       <c r="G24" s="34"/>
@@ -46712,9 +46783,9 @@
       <c r="J24" s="34"/>
       <c r="K24" s="34"/>
       <c r="L24" s="34"/>
-      <c r="M24" s="35" t="e">
+      <c r="M24" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="N24" s="34">
         <v>9</v>
@@ -46771,7 +46842,9 @@
       <c r="C25" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="34"/>
+      <c r="D25" s="34">
+        <v>10</v>
+      </c>
       <c r="E25" s="34"/>
       <c r="F25" s="34"/>
       <c r="G25" s="34"/>
@@ -46780,9 +46853,9 @@
       <c r="J25" s="34"/>
       <c r="K25" s="34"/>
       <c r="L25" s="34"/>
-      <c r="M25" s="35" t="e">
+      <c r="M25" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="N25" s="34">
         <v>9.5</v>
@@ -46839,7 +46912,9 @@
       <c r="C26" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="34"/>
+      <c r="D26" s="34">
+        <v>9</v>
+      </c>
       <c r="E26" s="34"/>
       <c r="F26" s="34"/>
       <c r="G26" s="34"/>
@@ -46848,9 +46923,9 @@
       <c r="J26" s="34"/>
       <c r="K26" s="34"/>
       <c r="L26" s="34"/>
-      <c r="M26" s="35" t="e">
+      <c r="M26" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>9</v>
       </c>
       <c r="N26" s="34">
         <v>10</v>
@@ -46907,7 +46982,9 @@
       <c r="C27" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="D27" s="34"/>
+      <c r="D27" s="34">
+        <v>2</v>
+      </c>
       <c r="E27" s="34"/>
       <c r="F27" s="34"/>
       <c r="G27" s="34"/>
@@ -46916,9 +46993,9 @@
       <c r="J27" s="34"/>
       <c r="K27" s="34"/>
       <c r="L27" s="34"/>
-      <c r="M27" s="35" t="e">
+      <c r="M27" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="N27" s="34">
         <v>10</v>
@@ -49503,11 +49580,11 @@
   <dimension ref="A1:AH200"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -49584,6 +49661,9 @@
       <c r="N4" s="15" t="s">
         <v>433</v>
       </c>
+      <c r="O4" s="15" t="s">
+        <v>466</v>
+      </c>
       <c r="U4" s="16"/>
       <c r="Y4" s="16"/>
       <c r="AC4" s="16"/>
@@ -49637,13 +49717,13 @@
       <c r="M6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="79"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="80"/>
-      <c r="Q6" s="80"/>
-      <c r="R6" s="80"/>
-      <c r="S6" s="80"/>
-      <c r="T6" s="81"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="31"/>
       <c r="U6" s="28" t="s">
         <v>10</v>
       </c>
@@ -49693,7 +49773,9 @@
       <c r="N7" s="34">
         <v>9.5</v>
       </c>
-      <c r="O7" s="34"/>
+      <c r="O7" s="34">
+        <v>10</v>
+      </c>
       <c r="P7" s="34"/>
       <c r="Q7" s="34"/>
       <c r="R7" s="34"/>
@@ -49701,7 +49783,7 @@
       <c r="T7" s="34"/>
       <c r="U7" s="35">
         <f>TRUNC(AVERAGE(N7:T7),2)</f>
-        <v>9.5</v>
+        <v>9.75</v>
       </c>
       <c r="V7" s="34"/>
       <c r="W7" s="34"/>
@@ -49763,7 +49845,9 @@
       <c r="N8" s="34">
         <v>10</v>
       </c>
-      <c r="O8" s="34"/>
+      <c r="O8" s="34">
+        <v>10</v>
+      </c>
       <c r="P8" s="34"/>
       <c r="Q8" s="34"/>
       <c r="R8" s="34"/>
@@ -49833,7 +49917,9 @@
       <c r="N9" s="34">
         <v>10</v>
       </c>
-      <c r="O9" s="34"/>
+      <c r="O9" s="34">
+        <v>10</v>
+      </c>
       <c r="P9" s="34"/>
       <c r="Q9" s="34"/>
       <c r="R9" s="34"/>
@@ -49903,7 +49989,9 @@
       <c r="N10" s="34">
         <v>10</v>
       </c>
-      <c r="O10" s="34"/>
+      <c r="O10" s="34">
+        <v>9.6</v>
+      </c>
       <c r="P10" s="34"/>
       <c r="Q10" s="34"/>
       <c r="R10" s="34"/>
@@ -49911,7 +49999,7 @@
       <c r="T10" s="34"/>
       <c r="U10" s="35">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="V10" s="34"/>
       <c r="W10" s="34"/>
@@ -49973,7 +50061,9 @@
       <c r="N11" s="34">
         <v>10</v>
       </c>
-      <c r="O11" s="34"/>
+      <c r="O11" s="34">
+        <v>10</v>
+      </c>
       <c r="P11" s="34"/>
       <c r="Q11" s="34"/>
       <c r="R11" s="34"/>
@@ -50043,7 +50133,9 @@
       <c r="N12" s="34">
         <v>10</v>
       </c>
-      <c r="O12" s="34"/>
+      <c r="O12" s="34">
+        <v>10</v>
+      </c>
       <c r="P12" s="34"/>
       <c r="Q12" s="34"/>
       <c r="R12" s="34"/>
@@ -50113,7 +50205,9 @@
       <c r="N13" s="34">
         <v>9.5</v>
       </c>
-      <c r="O13" s="34"/>
+      <c r="O13" s="34">
+        <v>8.4</v>
+      </c>
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
       <c r="R13" s="34"/>
@@ -50121,7 +50215,7 @@
       <c r="T13" s="34"/>
       <c r="U13" s="35">
         <f t="shared" si="3"/>
-        <v>9.5</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="V13" s="34"/>
       <c r="W13" s="34"/>
@@ -50183,7 +50277,9 @@
       <c r="N14" s="34">
         <v>9.5</v>
       </c>
-      <c r="O14" s="34"/>
+      <c r="O14" s="34">
+        <v>10</v>
+      </c>
       <c r="P14" s="34"/>
       <c r="Q14" s="34"/>
       <c r="R14" s="34"/>
@@ -50191,7 +50287,7 @@
       <c r="T14" s="34"/>
       <c r="U14" s="35">
         <f t="shared" si="3"/>
-        <v>9.5</v>
+        <v>9.75</v>
       </c>
       <c r="V14" s="34"/>
       <c r="W14" s="34"/>
@@ -50253,7 +50349,9 @@
       <c r="N15" s="34">
         <v>9.5</v>
       </c>
-      <c r="O15" s="34"/>
+      <c r="O15" s="34">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="P15" s="34"/>
       <c r="Q15" s="34"/>
       <c r="R15" s="34"/>
@@ -50261,7 +50359,7 @@
       <c r="T15" s="34"/>
       <c r="U15" s="35">
         <f t="shared" si="3"/>
-        <v>9.5</v>
+        <v>9.15</v>
       </c>
       <c r="V15" s="34"/>
       <c r="W15" s="34"/>
@@ -50323,7 +50421,9 @@
       <c r="N16" s="34">
         <v>9.5</v>
       </c>
-      <c r="O16" s="34"/>
+      <c r="O16" s="34" t="s">
+        <v>419</v>
+      </c>
       <c r="P16" s="34"/>
       <c r="Q16" s="34"/>
       <c r="R16" s="34"/>
@@ -50393,7 +50493,9 @@
       <c r="N17" s="34">
         <v>7</v>
       </c>
-      <c r="O17" s="34"/>
+      <c r="O17" s="34">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="P17" s="34"/>
       <c r="Q17" s="34"/>
       <c r="R17" s="34"/>
@@ -50401,7 +50503,7 @@
       <c r="T17" s="34"/>
       <c r="U17" s="35">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>7.6</v>
       </c>
       <c r="V17" s="34"/>
       <c r="W17" s="34"/>
@@ -50463,7 +50565,9 @@
       <c r="N18" s="34">
         <v>9.5</v>
       </c>
-      <c r="O18" s="34"/>
+      <c r="O18" s="34">
+        <v>9.8000000000000007</v>
+      </c>
       <c r="P18" s="34"/>
       <c r="Q18" s="34"/>
       <c r="R18" s="34"/>
@@ -50471,7 +50575,7 @@
       <c r="T18" s="34"/>
       <c r="U18" s="35">
         <f t="shared" si="3"/>
-        <v>9.5</v>
+        <v>9.65</v>
       </c>
       <c r="V18" s="34"/>
       <c r="W18" s="34"/>
@@ -50533,7 +50637,9 @@
       <c r="N19" s="34">
         <v>9</v>
       </c>
-      <c r="O19" s="34"/>
+      <c r="O19" s="34">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="P19" s="34"/>
       <c r="Q19" s="34"/>
       <c r="R19" s="34"/>
@@ -50541,7 +50647,7 @@
       <c r="T19" s="34"/>
       <c r="U19" s="35">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8.6</v>
       </c>
       <c r="V19" s="34"/>
       <c r="W19" s="34"/>
@@ -50603,7 +50709,9 @@
       <c r="N20" s="34">
         <v>9</v>
       </c>
-      <c r="O20" s="34"/>
+      <c r="O20" s="34">
+        <v>10</v>
+      </c>
       <c r="P20" s="34"/>
       <c r="Q20" s="34"/>
       <c r="R20" s="34"/>
@@ -50611,7 +50719,7 @@
       <c r="T20" s="34"/>
       <c r="U20" s="35">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="V20" s="34"/>
       <c r="W20" s="34"/>
@@ -50673,7 +50781,9 @@
       <c r="N21" s="34">
         <v>9.8000000000000007</v>
       </c>
-      <c r="O21" s="34"/>
+      <c r="O21" s="34">
+        <v>9</v>
+      </c>
       <c r="P21" s="34"/>
       <c r="Q21" s="34"/>
       <c r="R21" s="34"/>
@@ -50681,7 +50791,7 @@
       <c r="T21" s="34"/>
       <c r="U21" s="35">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>9.4</v>
       </c>
       <c r="V21" s="34"/>
       <c r="W21" s="34"/>
@@ -50743,7 +50853,9 @@
       <c r="N22" s="34">
         <v>10</v>
       </c>
-      <c r="O22" s="34"/>
+      <c r="O22" s="34">
+        <v>10</v>
+      </c>
       <c r="P22" s="34"/>
       <c r="Q22" s="34"/>
       <c r="R22" s="34"/>
@@ -50813,7 +50925,9 @@
       <c r="N23" s="34">
         <v>9.5</v>
       </c>
-      <c r="O23" s="34"/>
+      <c r="O23" s="34">
+        <v>10</v>
+      </c>
       <c r="P23" s="34"/>
       <c r="Q23" s="34"/>
       <c r="R23" s="34"/>
@@ -50821,7 +50935,7 @@
       <c r="T23" s="34"/>
       <c r="U23" s="35">
         <f t="shared" si="3"/>
-        <v>9.5</v>
+        <v>9.75</v>
       </c>
       <c r="V23" s="34"/>
       <c r="W23" s="34"/>
@@ -50883,7 +50997,9 @@
       <c r="N24" s="34">
         <v>10</v>
       </c>
-      <c r="O24" s="34"/>
+      <c r="O24" s="34">
+        <v>9.6</v>
+      </c>
       <c r="P24" s="34"/>
       <c r="Q24" s="34"/>
       <c r="R24" s="34"/>
@@ -50891,7 +51007,7 @@
       <c r="T24" s="34"/>
       <c r="U24" s="35">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="V24" s="34"/>
       <c r="W24" s="34"/>
@@ -50953,7 +51069,9 @@
       <c r="N25" s="34">
         <v>10</v>
       </c>
-      <c r="O25" s="34"/>
+      <c r="O25" s="34">
+        <v>10</v>
+      </c>
       <c r="P25" s="34"/>
       <c r="Q25" s="34"/>
       <c r="R25" s="34"/>
@@ -51023,7 +51141,9 @@
       <c r="N26" s="34">
         <v>8</v>
       </c>
-      <c r="O26" s="34"/>
+      <c r="O26" s="34">
+        <v>8</v>
+      </c>
       <c r="P26" s="34"/>
       <c r="Q26" s="34"/>
       <c r="R26" s="34"/>
@@ -51093,7 +51213,9 @@
       <c r="N27" s="34">
         <v>8</v>
       </c>
-      <c r="O27" s="34"/>
+      <c r="O27" s="34">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="P27" s="34"/>
       <c r="Q27" s="34"/>
       <c r="R27" s="34"/>
@@ -51101,7 +51223,7 @@
       <c r="T27" s="34"/>
       <c r="U27" s="35">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>8.1</v>
       </c>
       <c r="V27" s="34"/>
       <c r="W27" s="34"/>
@@ -53654,9 +53776,6 @@
       <c r="AH200" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="N6:T6"/>
-  </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.19685039370078741" top="0.59055118110236227" bottom="0.78740157480314965" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -53672,7 +53791,7 @@
   </sheetPr>
   <dimension ref="A1:AH200"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B7" sqref="B7:C28"/>
       <selection pane="topRight" activeCell="B7" sqref="B7:C28"/>
@@ -62190,7 +62309,7 @@
       <c r="AF3" s="12"/>
       <c r="AG3" s="12"/>
     </row>
-    <row r="4" spans="1:34" s="15" customFormat="1" ht="156">
+    <row r="4" spans="1:34" s="15" customFormat="1" ht="155.25">
       <c r="A4" s="14"/>
       <c r="M4" s="16"/>
       <c r="N4" s="15" t="s">
@@ -70669,7 +70788,7 @@
       <c r="AG3" s="12"/>
       <c r="AH3" s="12"/>
     </row>
-    <row r="4" spans="1:35" s="15" customFormat="1" ht="170.25">
+    <row r="4" spans="1:35" s="15" customFormat="1" ht="169.5">
       <c r="A4" s="14"/>
       <c r="D4" s="15" t="s">
         <v>424</v>

</xml_diff>